<commit_message>
fixes, debugs and improvements
</commit_message>
<xml_diff>
--- a/agentic_clarifycoder/results.xlsx
+++ b/agentic_clarifycoder/results.xlsx
@@ -476,23 +476,35 @@
           <t>baseline</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>26.67</v>
-      </c>
-      <c r="C2" t="n">
-        <v>50</v>
-      </c>
-      <c r="D2" t="n">
-        <v>50</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>26.67</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>(0.0, 0)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>(100.0, 0)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>(0, 0)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>(0, 0)</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>(0.0, 0)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>(100.0, 0)</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -501,23 +513,35 @@
           <t>llm</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>46.67</v>
-      </c>
-      <c r="C3" t="n">
-        <v>65.56</v>
-      </c>
-      <c r="D3" t="n">
-        <v>65.56</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>56.67</v>
-      </c>
-      <c r="G3" t="n">
-        <v>43.33</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>(0.0, 0)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>(100.0, 0)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>(0, 0)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>(0, 0)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>(0.0, 0)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>(100.0, 0)</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -526,23 +550,35 @@
           <t>hybrid</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>43.33</v>
-      </c>
-      <c r="C4" t="n">
-        <v>24.44</v>
-      </c>
-      <c r="D4" t="n">
-        <v>24.44</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>6.67</v>
-      </c>
-      <c r="G4" t="n">
-        <v>30</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>(0.0, 0)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>(100.0, 0)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>(0, 0)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>(0, 0)</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>(0.0, 0)</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>(100.0, 0)</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>